<commit_message>
feature: email function init
</commit_message>
<xml_diff>
--- a/main_database_MU.xlsx
+++ b/main_database_MU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fahimhadimaula/Documents/F01 - YDL Generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD15454-2F01-FD4E-A106-726F13A58E82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CED2EE-157E-B040-9CDB-4F7DE36CD988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16620" firstSheet="1" activeTab="6" xr2:uid="{81325CCC-8403-1346-9F67-FB9C5372A5A0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" activeTab="1" xr2:uid="{81325CCC-8403-1346-9F67-FB9C5372A5A0}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="162">
   <si>
     <t>event_name</t>
   </si>
@@ -198,9 +198,6 @@
     <t>M Rizka Fadhli</t>
   </si>
   <si>
-    <t>rizka.fadhli@nutrifood.co.id</t>
-  </si>
-  <si>
     <t>Andhika Surya</t>
   </si>
   <si>
@@ -234,30 +231,6 @@
     <t>SQA</t>
   </si>
   <si>
-    <t>Andhika.Surya@nutrifood.co.id</t>
-  </si>
-  <si>
-    <t>doniafrizalisnan96@gmail.com</t>
-  </si>
-  <si>
-    <t>riswanalamsyah12@gmail.com</t>
-  </si>
-  <si>
-    <t>galang080101@gmail.com</t>
-  </si>
-  <si>
-    <t>alfiah.nur@nutrifood.co.id</t>
-  </si>
-  <si>
-    <t>zadkielsieghart@gmail.com</t>
-  </si>
-  <si>
-    <t>Handikadaihatsu@gmail.com</t>
-  </si>
-  <si>
-    <t>Saeful.Ihsan468@gmail.com</t>
-  </si>
-  <si>
     <t>NIK</t>
   </si>
   <si>
@@ -535,6 +508,21 @@
   </si>
   <si>
     <t>conclusion</t>
+  </si>
+  <si>
+    <t>Hasmy Halid</t>
+  </si>
+  <si>
+    <t>hasmy_h@nutrifood.co.id</t>
+  </si>
+  <si>
+    <t>fahimhadimaula@gmail.com</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>prameswari.kristal@nutrifood.co.id</t>
   </si>
 </sst>
 </file>
@@ -909,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF422842-D907-E645-8D38-10578ACC7467}">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -956,7 +944,7 @@
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="J1" t="s">
         <v>17</v>
@@ -968,10 +956,10 @@
         <v>50</v>
       </c>
       <c r="M1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="O1" t="s">
         <v>18</v>
@@ -1005,7 +993,7 @@
         <v>120</v>
       </c>
       <c r="I2" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="J2" s="4" t="str">
         <f>"C"&amp;TEXT(ROW(A2)-1,"0000")</f>
@@ -1048,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F384A96-5D36-5A4B-ACC6-02F83627BA9A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1086,7 +1074,7 @@
         <v>52</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1098,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1C9A2A-128B-BF45-A10E-8734AF0ABDEC}">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1135,13 +1123,13 @@
         <v>17</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -1162,46 +1150,46 @@
         <v>47</v>
       </c>
       <c r="M1" t="s">
+        <v>131</v>
+      </c>
+      <c r="N1" t="s">
+        <v>132</v>
+      </c>
+      <c r="O1" t="s">
+        <v>133</v>
+      </c>
+      <c r="P1" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>135</v>
+      </c>
+      <c r="R1" t="s">
+        <v>136</v>
+      </c>
+      <c r="S1" t="s">
+        <v>137</v>
+      </c>
+      <c r="T1" t="s">
+        <v>138</v>
+      </c>
+      <c r="U1" t="s">
+        <v>139</v>
+      </c>
+      <c r="V1" t="s">
         <v>140</v>
       </c>
-      <c r="N1" t="s">
+      <c r="W1" t="s">
         <v>141</v>
       </c>
-      <c r="O1" t="s">
+      <c r="X1" t="s">
         <v>142</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Y1" t="s">
         <v>143</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Z1" t="s">
         <v>144</v>
-      </c>
-      <c r="R1" t="s">
-        <v>145</v>
-      </c>
-      <c r="S1" t="s">
-        <v>146</v>
-      </c>
-      <c r="T1" t="s">
-        <v>147</v>
-      </c>
-      <c r="U1" t="s">
-        <v>148</v>
-      </c>
-      <c r="V1" t="s">
-        <v>149</v>
-      </c>
-      <c r="W1" t="s">
-        <v>150</v>
-      </c>
-      <c r="X1" t="s">
-        <v>151</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>152</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
@@ -1220,16 +1208,16 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" t="s">
-        <v>65</v>
+        <v>160</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="I2" t="s">
         <v>39</v>
@@ -1238,7 +1226,7 @@
         <v>42</v>
       </c>
       <c r="L2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
@@ -1257,16 +1245,16 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" t="s">
-        <v>36</v>
+        <v>160</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="I3" t="s">
         <v>39</v>
@@ -1275,7 +1263,7 @@
         <v>42</v>
       </c>
       <c r="L3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
@@ -1294,16 +1282,16 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
-        <v>66</v>
+        <v>160</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="I4" t="s">
         <v>39</v>
@@ -1312,7 +1300,7 @@
         <v>42</v>
       </c>
       <c r="L4" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
@@ -1331,16 +1319,16 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>67</v>
+        <v>160</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="I5" t="s">
         <v>39</v>
@@ -1349,7 +1337,7 @@
         <v>42</v>
       </c>
       <c r="L5" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
@@ -1368,16 +1356,16 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" t="s">
-        <v>68</v>
+        <v>160</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="I6" t="s">
         <v>39</v>
@@ -1386,7 +1374,7 @@
         <v>42</v>
       </c>
       <c r="L6" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
@@ -1405,16 +1393,16 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G7" t="s">
-        <v>64</v>
-      </c>
-      <c r="H7" t="s">
-        <v>69</v>
+        <v>160</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="I7" t="s">
         <v>39</v>
@@ -1423,7 +1411,7 @@
         <v>42</v>
       </c>
       <c r="L7" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
@@ -1442,16 +1430,16 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" t="s">
-        <v>36</v>
+        <v>160</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="I8" t="s">
         <v>39</v>
@@ -1460,7 +1448,7 @@
         <v>42</v>
       </c>
       <c r="L8" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
@@ -1479,16 +1467,16 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F9" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" t="s">
-        <v>70</v>
+        <v>160</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="I9" t="s">
         <v>40</v>
@@ -1500,7 +1488,7 @@
         <v>42</v>
       </c>
       <c r="L9" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
@@ -1519,16 +1507,16 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" t="s">
-        <v>71</v>
+        <v>160</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="I10" t="s">
         <v>40</v>
@@ -1540,7 +1528,7 @@
         <v>42</v>
       </c>
       <c r="L10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
@@ -1559,16 +1547,16 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F11" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="G11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" t="s">
-        <v>72</v>
+        <v>160</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="I11" t="s">
         <v>40</v>
@@ -1580,7 +1568,7 @@
         <v>42</v>
       </c>
       <c r="L11" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1593,7 +1581,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1631,7 +1619,7 @@
         <v>POK | Basic Statistic</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D2" s="4" t="str">
         <f>INDEX(room_list!$B$1:$B$60,MATCH(training_room!$C2,room_list!$A$1:$A$60,0))</f>
@@ -1663,8 +1651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BDC3934-0582-6147-B812-92202E769732}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1683,31 +1671,31 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I1" t="s">
         <v>154</v>
       </c>
-      <c r="D1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G1" t="s">
-        <v>161</v>
-      </c>
-      <c r="H1" t="s">
-        <v>162</v>
-      </c>
-      <c r="I1" t="s">
-        <v>163</v>
-      </c>
       <c r="J1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="K1" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1719,7 +1707,7 @@
         <v>POK | Basic Statistic</v>
       </c>
       <c r="C2" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1729,10 +1717,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB334BD1-1ED9-EC44-8A3B-500E9A56F3BA}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1811,6 +1799,20 @@
         <v>38</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1820,7 +1822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F17FBF25-33A8-1548-B4A6-1E41965F60FD}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
@@ -1832,7 +1834,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C1" t="s">
         <v>28</v>
@@ -1840,7 +1842,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
@@ -1848,7 +1850,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -1856,7 +1858,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
@@ -1864,7 +1866,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
@@ -1872,7 +1874,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
         <v>28</v>
@@ -1880,7 +1882,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
         <v>28</v>
@@ -1888,7 +1890,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s">
         <v>28</v>
@@ -1896,7 +1898,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
         <v>28</v>
@@ -1904,7 +1906,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
         <v>28</v>
@@ -1912,7 +1914,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
         <v>28</v>
@@ -1920,7 +1922,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
         <v>28</v>
@@ -1928,7 +1930,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
@@ -1936,7 +1938,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C14" t="s">
         <v>28</v>
@@ -1944,7 +1946,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C15" t="s">
         <v>28</v>
@@ -1952,7 +1954,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s">
         <v>28</v>
@@ -1960,7 +1962,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
         <v>28</v>
@@ -1976,7 +1978,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C19" t="s">
         <v>28</v>
@@ -1984,10 +1986,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
         <v>28</v>
@@ -1995,7 +1997,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
         <v>28</v>
@@ -2003,7 +2005,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C22" t="s">
         <v>28</v>
@@ -2011,7 +2013,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C23" t="s">
         <v>28</v>
@@ -2019,7 +2021,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
@@ -2027,7 +2029,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
         <v>28</v>
@@ -2035,7 +2037,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C26" t="s">
         <v>28</v>
@@ -2043,7 +2045,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
         <v>28</v>
@@ -2051,7 +2053,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C28" t="s">
         <v>28</v>
@@ -2059,7 +2061,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
         <v>28</v>
@@ -2067,7 +2069,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C30" t="s">
         <v>28</v>
@@ -2075,7 +2077,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C31" t="s">
         <v>28</v>
@@ -2083,7 +2085,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C32" t="s">
         <v>28</v>
@@ -2091,7 +2093,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C33" t="s">
         <v>28</v>
@@ -2099,7 +2101,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C34" t="s">
         <v>28</v>
@@ -2107,7 +2109,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C35" t="s">
         <v>28</v>
@@ -2115,7 +2117,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C36" t="s">
         <v>28</v>
@@ -2123,7 +2125,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C37" t="s">
         <v>28</v>
@@ -2131,7 +2133,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C38" t="s">
         <v>28</v>
@@ -2139,7 +2141,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C39" t="s">
         <v>28</v>
@@ -2147,7 +2149,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C40" t="s">
         <v>28</v>
@@ -2155,7 +2157,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C41" t="s">
         <v>28</v>
@@ -2163,7 +2165,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C42" t="s">
         <v>28</v>
@@ -2171,7 +2173,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C43" t="s">
         <v>28</v>
@@ -2179,7 +2181,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C44" t="s">
         <v>28</v>
@@ -2187,7 +2189,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C45" t="s">
         <v>28</v>
@@ -2195,7 +2197,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C46" t="s">
         <v>28</v>
@@ -2203,7 +2205,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C47" t="s">
         <v>28</v>
@@ -2211,7 +2213,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C48" t="s">
         <v>28</v>
@@ -2219,7 +2221,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C49" t="s">
         <v>28</v>
@@ -2227,7 +2229,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C50" t="s">
         <v>28</v>
@@ -2235,7 +2237,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C51" t="s">
         <v>28</v>
@@ -2243,7 +2245,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C52" t="s">
         <v>28</v>
@@ -2251,7 +2253,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C53" t="s">
         <v>28</v>
@@ -2259,7 +2261,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C54" t="s">
         <v>28</v>
@@ -2267,7 +2269,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C55" t="s">
         <v>28</v>
@@ -2275,42 +2277,42 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C56" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C57" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C58" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C59" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C60" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug resolved: read excel formulas as value
</commit_message>
<xml_diff>
--- a/main_database_MU.xlsx
+++ b/main_database_MU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fahimhadimaula/Documents/F01 - YDL Generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF45D7F-A010-7140-92E6-E46072095995}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCC1D21-6124-7144-9EFF-CEF09B88E3A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="163">
   <si>
     <t>event_code</t>
   </si>
@@ -286,12 +286,6 @@
   </si>
   <si>
     <t>cc_3</t>
-  </si>
-  <si>
-    <t>cc_4</t>
-  </si>
-  <si>
-    <t>cc_5</t>
   </si>
   <si>
     <t>GLF</t>
@@ -902,7 +896,7 @@
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1093,8 +1087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1117,10 +1111,6 @@
     <col min="17" max="17" width="15.5" style="4" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
@@ -1724,10 +1714,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1738,7 +1728,7 @@
     <col min="5" max="5" width="37" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1754,76 +1744,70 @@
       <c r="E1" t="s">
         <v>83</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>84</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>86</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>87</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>88</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>89</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>91</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>92</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>93</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>94</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B4" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" t="s">
         <v>96</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>97</v>
       </c>
-      <c r="C4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>98</v>
       </c>
-      <c r="E4" t="s">
+      <c r="B5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
         <v>100</v>
       </c>
-      <c r="B5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" t="s">
-        <v>102</v>
-      </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1847,154 +1831,154 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2002,330 +1986,330 @@
         <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C34" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C35" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C38" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C39" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C41" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C42" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C43" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C44" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C45" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C46" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C48" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C49" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C50" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C51" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C52" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C53" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C54" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C55" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C56" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C57" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C58" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C59" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C60" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>